<commit_message>
Ref and Dev guides updated, Sample project and Tutorial 7 fixed
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.demo/src/org.openl.rules.demo.tutorials/Tutorial 7 - Introduction to Table Properties/Tutorial7 - Intro to Table Properties.xlsx
+++ b/STUDIO/org.openl.rules.demo/src/org.openl.rules.demo.tutorials/Tutorial 7 - Introduction to Table Properties/Tutorial7 - Intro to Table Properties.xlsx
@@ -27,6 +27,45 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Property name. "modifiedOn" property indicates the date of the last table modification in OpenL
+Tablets WebStudio.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Property value</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -92,7 +131,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -131,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="150">
   <si>
     <t>Amount</t>
   </si>
@@ -1166,6 +1205,9 @@
   </si>
   <si>
     <t>Test CarPrice CarPrice2009Test</t>
+  </si>
+  <si>
+    <t>modifiedOn</t>
   </si>
 </sst>
 </file>
@@ -1875,7 +1917,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -2074,6 +2116,9 @@
     <xf numFmtId="14" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2116,15 +2161,42 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="21" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2140,33 +2212,6 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="21" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2176,6 +2221,10 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Heading 1 2" xfId="9"/>
@@ -2287,13 +2336,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1400175</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2761,16 +2810,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
@@ -2812,64 +2861,64 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -2934,72 +2983,72 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="79" t="s">
+      <c r="C18" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -3070,8 +3119,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3113,18 +3162,18 @@
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3143,74 +3192,74 @@
     </row>
     <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -3229,31 +3278,33 @@
     </row>
     <row r="24" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
-      <c r="C24" s="80" t="s">
+      <c r="C24" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="108">
+        <v>41313.03170702546</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -3261,10 +3312,10 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="14">
-        <v>0.7</v>
+        <v>79</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3272,10 +3323,10 @@
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="14">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -3283,10 +3334,10 @@
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="14">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3294,10 +3345,10 @@
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="14">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -3305,29 +3356,33 @@
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" s="14">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
-      <c r="C32" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="15">
-        <v>0.95</v>
+      <c r="C32" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="C33" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="15">
+        <v>0.95</v>
+      </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
@@ -3340,60 +3395,60 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
-      <c r="C35" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
-      <c r="C36" s="82"/>
+      <c r="C36" s="82" t="s">
+        <v>87</v>
+      </c>
       <c r="D36" s="82"/>
       <c r="E36" s="82"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
+      <c r="C42" s="83"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="83"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -3405,9 +3460,9 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -3424,19 +3479,19 @@
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
-      <c r="C47" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="12"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
+      <c r="C48" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="12"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
@@ -3447,19 +3502,27 @@
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
     </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C35:E43"/>
+    <mergeCell ref="C36:E44"/>
     <mergeCell ref="C12:E21"/>
     <mergeCell ref="C8:E9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C47" location="_st2" tooltip="Step2. Business Dimensional Properties. Versioning by properties" display="Step 2."/>
+    <hyperlink ref="C48" location="_st2" tooltip="Step2. Business Dimensional Properties. Versioning by properties" display="Step 2."/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3524,11 +3587,11 @@
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -3540,9 +3603,9 @@
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -3582,13 +3645,13 @@
     <row r="12" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -3598,11 +3661,11 @@
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -3612,11 +3675,11 @@
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -3626,11 +3689,11 @@
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -3640,11 +3703,11 @@
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -3654,11 +3717,11 @@
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -3668,11 +3731,11 @@
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -3682,11 +3745,11 @@
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -3724,13 +3787,13 @@
     <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="81" t="s">
+      <c r="D22" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3740,11 +3803,11 @@
     <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -3754,11 +3817,11 @@
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -3768,11 +3831,11 @@
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3809,23 +3872,23 @@
     </row>
     <row r="28" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
-      <c r="C29" s="101" t="s">
+      <c r="C29" s="95" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="65" t="s">
@@ -3845,7 +3908,7 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
-      <c r="C30" s="101"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="65" t="s">
         <v>37</v>
       </c>
@@ -3933,35 +3996,35 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
-      <c r="C34" s="97" t="s">
+      <c r="C34" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="97" t="s">
+      <c r="D34" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="87" t="s">
+      <c r="E34" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="99" t="s">
+      <c r="F34" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="100"/>
-      <c r="H34" s="100" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I34" s="100"/>
-      <c r="J34" s="100"/>
-      <c r="K34" s="100" t="s">
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="L34" s="102"/>
+      <c r="L34" s="96"/>
       <c r="M34" s="9"/>
     </row>
     <row r="35" spans="2:13" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="9"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="98"/>
-      <c r="E35" s="88"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="94"/>
       <c r="F35" s="25" t="s">
         <v>18</v>
       </c>
@@ -3990,7 +4053,7 @@
       <c r="C36" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="94" t="s">
+      <c r="D36" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="28" t="s">
@@ -4024,7 +4087,7 @@
       <c r="C37" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="95"/>
+      <c r="D37" s="87"/>
       <c r="E37" s="23" t="s">
         <v>30</v>
       </c>
@@ -4056,7 +4119,7 @@
       <c r="C38" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="95"/>
+      <c r="D38" s="87"/>
       <c r="E38" s="23" t="s">
         <v>31</v>
       </c>
@@ -4088,7 +4151,7 @@
       <c r="C39" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="95" t="s">
+      <c r="D39" s="87" t="s">
         <v>24</v>
       </c>
       <c r="E39" s="23" t="s">
@@ -4122,7 +4185,7 @@
       <c r="C40" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="23" t="s">
         <v>27</v>
       </c>
@@ -4154,7 +4217,7 @@
       <c r="C41" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="95"/>
+      <c r="D41" s="87"/>
       <c r="E41" s="23" t="s">
         <v>28</v>
       </c>
@@ -4186,7 +4249,7 @@
       <c r="C42" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="95" t="s">
+      <c r="D42" s="87" t="s">
         <v>25</v>
       </c>
       <c r="E42" s="23" t="s">
@@ -4220,7 +4283,7 @@
       <c r="C43" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="95"/>
+      <c r="D43" s="87"/>
       <c r="E43" s="23" t="s">
         <v>33</v>
       </c>
@@ -4252,7 +4315,7 @@
       <c r="C44" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="96"/>
+      <c r="D44" s="88"/>
       <c r="E44" s="24" t="s">
         <v>34</v>
       </c>
@@ -4309,23 +4372,23 @@
     </row>
     <row r="47" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
-      <c r="C47" s="80" t="s">
+      <c r="C47" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="80"/>
-      <c r="L47" s="80"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="81"/>
+      <c r="K47" s="81"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="9"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
-      <c r="C48" s="101" t="s">
+      <c r="C48" s="95" t="s">
         <v>35</v>
       </c>
       <c r="D48" s="65" t="s">
@@ -4345,7 +4408,7 @@
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="9"/>
-      <c r="C49" s="101"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="65" t="s">
         <v>37</v>
       </c>
@@ -4433,43 +4496,43 @@
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="9"/>
-      <c r="C53" s="97" t="s">
+      <c r="C53" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="97" t="s">
+      <c r="D53" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="87" t="s">
+      <c r="E53" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="99" t="s">
+      <c r="F53" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="G53" s="100" t="s">
+      <c r="G53" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="100" t="s">
+      <c r="H53" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="100" t="s">
+      <c r="I53" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="100" t="s">
+      <c r="J53" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="K53" s="100" t="s">
+      <c r="K53" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="L53" s="102" t="s">
+      <c r="L53" s="96" t="s">
         <v>15</v>
       </c>
       <c r="M53" s="9"/>
     </row>
     <row r="54" spans="2:13" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="9"/>
-      <c r="C54" s="98"/>
-      <c r="D54" s="98"/>
-      <c r="E54" s="88"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="92"/>
+      <c r="E54" s="94"/>
       <c r="F54" s="25" t="s">
         <v>18</v>
       </c>
@@ -4498,7 +4561,7 @@
       <c r="C55" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="94" t="s">
+      <c r="D55" s="97" t="s">
         <v>23</v>
       </c>
       <c r="E55" s="28" t="s">
@@ -4532,7 +4595,7 @@
       <c r="C56" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="95" t="s">
+      <c r="D56" s="87" t="s">
         <v>23</v>
       </c>
       <c r="E56" s="23" t="s">
@@ -4566,7 +4629,7 @@
       <c r="C57" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="95" t="s">
+      <c r="D57" s="87" t="s">
         <v>23</v>
       </c>
       <c r="E57" s="23" t="s">
@@ -4600,7 +4663,7 @@
       <c r="C58" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="D58" s="95" t="s">
+      <c r="D58" s="87" t="s">
         <v>24</v>
       </c>
       <c r="E58" s="23" t="s">
@@ -4634,7 +4697,7 @@
       <c r="C59" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="D59" s="95" t="s">
+      <c r="D59" s="87" t="s">
         <v>24</v>
       </c>
       <c r="E59" s="23" t="s">
@@ -4668,7 +4731,7 @@
       <c r="C60" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="95" t="s">
+      <c r="D60" s="87" t="s">
         <v>24</v>
       </c>
       <c r="E60" s="23" t="s">
@@ -4702,7 +4765,7 @@
       <c r="C61" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D61" s="95" t="s">
+      <c r="D61" s="87" t="s">
         <v>25</v>
       </c>
       <c r="E61" s="23" t="s">
@@ -4736,7 +4799,7 @@
       <c r="C62" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="D62" s="95" t="s">
+      <c r="D62" s="87" t="s">
         <v>25</v>
       </c>
       <c r="E62" s="23" t="s">
@@ -4770,7 +4833,7 @@
       <c r="C63" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="96" t="s">
+      <c r="D63" s="88" t="s">
         <v>25</v>
       </c>
       <c r="E63" s="24" t="s">
@@ -4830,13 +4893,13 @@
     <row r="66" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
-      <c r="D66" s="80" t="s">
+      <c r="D66" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="E66" s="80"/>
-      <c r="F66" s="80"/>
-      <c r="G66" s="80"/>
-      <c r="H66" s="80"/>
+      <c r="E66" s="81"/>
+      <c r="F66" s="81"/>
+      <c r="G66" s="81"/>
+      <c r="H66" s="81"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5100,11 +5163,11 @@
     <row r="79" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
-      <c r="D79" s="89" t="s">
+      <c r="D79" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="E79" s="89"/>
-      <c r="F79" s="89"/>
+      <c r="E79" s="99"/>
+      <c r="F79" s="99"/>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
@@ -5119,10 +5182,10 @@
       <c r="D80" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="E80" s="90" t="s">
+      <c r="E80" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="F80" s="90"/>
+      <c r="F80" s="100"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
@@ -5137,10 +5200,10 @@
       <c r="D81" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="E81" s="91" t="s">
+      <c r="E81" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="F81" s="91"/>
+      <c r="F81" s="101"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
@@ -5155,10 +5218,10 @@
       <c r="D82" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E82" s="91" t="s">
+      <c r="E82" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="F82" s="91"/>
+      <c r="F82" s="101"/>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
       <c r="I82" s="9"/>
@@ -5173,10 +5236,10 @@
       <c r="D83" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E83" s="91" t="s">
+      <c r="E83" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="F83" s="91"/>
+      <c r="F83" s="101"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
@@ -5191,10 +5254,10 @@
       <c r="D84" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="E84" s="92" t="s">
+      <c r="E84" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="F84" s="92"/>
+      <c r="F84" s="102"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
@@ -5209,10 +5272,10 @@
       <c r="D85" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E85" s="93" t="s">
+      <c r="E85" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="F85" s="93"/>
+      <c r="F85" s="103"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>
@@ -5296,10 +5359,10 @@
     <row r="91" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
-      <c r="D91" s="86" t="s">
+      <c r="D91" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="86" t="s">
+      <c r="E91" s="98" t="s">
         <v>71</v>
       </c>
       <c r="F91" s="9"/>
@@ -5378,10 +5441,10 @@
     <row r="96" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
-      <c r="D96" s="86" t="s">
+      <c r="D96" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="E96" s="86"/>
+      <c r="E96" s="98"/>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
@@ -5656,13 +5719,13 @@
     <row r="114" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="81" t="s">
+      <c r="D114" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="E114" s="81"/>
-      <c r="F114" s="81"/>
-      <c r="G114" s="81"/>
-      <c r="H114" s="81"/>
+      <c r="E114" s="82"/>
+      <c r="F114" s="82"/>
+      <c r="G114" s="82"/>
+      <c r="H114" s="82"/>
       <c r="I114" s="9"/>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
@@ -5672,11 +5735,11 @@
     <row r="115" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
-      <c r="D115" s="82"/>
-      <c r="E115" s="82"/>
-      <c r="F115" s="82"/>
-      <c r="G115" s="82"/>
-      <c r="H115" s="82"/>
+      <c r="D115" s="83"/>
+      <c r="E115" s="83"/>
+      <c r="F115" s="83"/>
+      <c r="G115" s="83"/>
+      <c r="H115" s="83"/>
       <c r="I115" s="9"/>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
@@ -5686,11 +5749,11 @@
     <row r="116" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
-      <c r="D116" s="83"/>
-      <c r="E116" s="83"/>
-      <c r="F116" s="83"/>
-      <c r="G116" s="83"/>
-      <c r="H116" s="83"/>
+      <c r="D116" s="84"/>
+      <c r="E116" s="84"/>
+      <c r="F116" s="84"/>
+      <c r="G116" s="84"/>
+      <c r="H116" s="84"/>
       <c r="I116" s="9"/>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
@@ -5725,16 +5788,16 @@
       <c r="L118" s="9"/>
       <c r="M118" s="9"/>
     </row>
-    <row r="119" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
-      <c r="D119" s="80" t="s">
+      <c r="D119" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="E119" s="80"/>
-      <c r="F119" s="80"/>
-      <c r="G119" s="80"/>
-      <c r="H119" s="80"/>
+      <c r="E119" s="81"/>
+      <c r="F119" s="81"/>
+      <c r="G119" s="81"/>
+      <c r="H119" s="81"/>
       <c r="I119" s="9"/>
       <c r="J119" s="9"/>
       <c r="K119" s="9"/>
@@ -5979,15 +6042,15 @@
       <c r="L130" s="9"/>
       <c r="M130" s="9"/>
     </row>
-    <row r="131" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
-      <c r="D131" s="80" t="s">
+      <c r="D131" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="E131" s="80"/>
-      <c r="F131" s="80"/>
-      <c r="G131" s="80"/>
+      <c r="E131" s="81"/>
+      <c r="F131" s="81"/>
+      <c r="G131" s="81"/>
       <c r="H131" s="9"/>
       <c r="I131" s="9"/>
       <c r="J131" s="9"/>
@@ -6182,11 +6245,11 @@
     <row r="142" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
-      <c r="D142" s="80" t="s">
+      <c r="D142" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="E142" s="80"/>
-      <c r="F142" s="80"/>
+      <c r="E142" s="81"/>
+      <c r="F142" s="81"/>
       <c r="G142" s="9"/>
       <c r="H142" s="9"/>
       <c r="I142" s="9"/>
@@ -6406,10 +6469,10 @@
     <row r="154" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
-      <c r="D154" s="80" t="s">
+      <c r="D154" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="E154" s="80"/>
+      <c r="E154" s="81"/>
       <c r="F154" s="9"/>
       <c r="G154" s="9"/>
       <c r="H154" s="9"/>
@@ -6633,25 +6696,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="D12:H19"/>
-    <mergeCell ref="D22:H25"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D119:H119"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D114:H116"/>
+    <mergeCell ref="D131:G131"/>
     <mergeCell ref="D8:F9"/>
     <mergeCell ref="D96:E96"/>
     <mergeCell ref="E53:E54"/>
@@ -6668,11 +6717,25 @@
     <mergeCell ref="D58:D60"/>
     <mergeCell ref="D61:D63"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D119:H119"/>
-    <mergeCell ref="D142:F142"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D114:H116"/>
-    <mergeCell ref="D131:G131"/>
+    <mergeCell ref="D12:H19"/>
+    <mergeCell ref="D22:H25"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K34:L34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D165" location="_st3" tooltip="Step3. Category and Module Level Properties" display="Step 3."/>
@@ -6735,11 +6798,11 @@
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6747,9 +6810,9 @@
     </row>
     <row r="9" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -6777,11 +6840,11 @@
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -6789,9 +6852,9 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -6799,9 +6862,9 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -6809,9 +6872,9 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -6869,11 +6932,11 @@
     </row>
     <row r="21" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
-      <c r="C21" s="104" t="s">
+      <c r="C21" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -6901,11 +6964,11 @@
     </row>
     <row r="24" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
-      <c r="C24" s="81" t="s">
+      <c r="C24" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -6913,9 +6976,9 @@
     </row>
     <row r="25" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -6923,9 +6986,9 @@
     </row>
     <row r="26" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -6933,9 +6996,9 @@
     </row>
     <row r="27" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -6943,9 +7006,9 @@
     </row>
     <row r="28" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -6953,9 +7016,9 @@
     </row>
     <row r="29" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -6963,9 +7026,9 @@
     </row>
     <row r="30" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -6973,9 +7036,9 @@
     </row>
     <row r="31" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -7003,10 +7066,10 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
-      <c r="C34" s="105" t="s">
+      <c r="C34" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="D34" s="105"/>
+      <c r="D34" s="106"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -7107,11 +7170,11 @@
     </row>
     <row r="43" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
-      <c r="C43" s="104" t="s">
+      <c r="C43" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="104"/>
-      <c r="E43" s="104"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -7139,11 +7202,11 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
@@ -7151,9 +7214,9 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
+      <c r="C47" s="83"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="83"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -7161,9 +7224,9 @@
     </row>
     <row r="48" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -7171,9 +7234,9 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="9"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
+      <c r="C49" s="83"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -7181,9 +7244,9 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="9"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
+      <c r="C50" s="83"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -7191,9 +7254,9 @@
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="9"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -7221,11 +7284,11 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="9"/>
-      <c r="C54" s="81" t="s">
+      <c r="C54" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="82"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -7233,9 +7296,9 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
-      <c r="E55" s="82"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -7243,9 +7306,9 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="82"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="83"/>
+      <c r="E56" s="83"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
@@ -7253,9 +7316,9 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="83"/>
+      <c r="E57" s="83"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -7263,9 +7326,9 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
-      <c r="C58" s="83"/>
-      <c r="D58" s="83"/>
-      <c r="E58" s="83"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -7423,11 +7486,11 @@
     </row>
     <row r="74" spans="2:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
-      <c r="C74" s="103" t="s">
+      <c r="C74" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="103"/>
-      <c r="E74" s="103"/>
+      <c r="D74" s="104"/>
+      <c r="E74" s="104"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>

</xml_diff>